<commit_message>
On the GAE side: fetch_all() and get() work. Also display work. On local server side: publish(), fetch_all() and load_template() works.
</commit_message>
<xml_diff>
--- a/spreadsheets/PublishAList.xlsx
+++ b/spreadsheets/PublishAList.xlsx
@@ -12,7 +12,10 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="11655" windowHeight="6270"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Data" sheetId="1" r:id="rId1"/>
+    <sheet name="Data.AQ" sheetId="8" r:id="rId2"/>
+    <sheet name="Configuration" sheetId="7" r:id="rId3"/>
+    <sheet name="Data.AQ2" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="94">
   <si>
     <t>Jan</t>
   </si>
@@ -42,13 +45,277 @@
   </si>
   <si>
     <t>Mikke</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>ABB Banks</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>List</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>It's a list of banks which ABB has a relationship with(deposits, derivatives, guarantees, letters of credit).</t>
+  </si>
+  <si>
+    <t>Created by</t>
+  </si>
+  <si>
+    <t>bartosz.piechnik@ch.abb.com</t>
+  </si>
+  <si>
+    <t>_ApplyTypes_</t>
+  </si>
+  <si>
+    <t>_FlagAsMethod</t>
+  </si>
+  <si>
+    <t>_LazyAddAttr_</t>
+  </si>
+  <si>
+    <t>_NewEnum</t>
+  </si>
+  <si>
+    <t>_Release_</t>
+  </si>
+  <si>
+    <t>__AttrToID__</t>
+  </si>
+  <si>
+    <t>__LazyMap__</t>
+  </si>
+  <si>
+    <t>__call__</t>
+  </si>
+  <si>
+    <t>__doc__</t>
+  </si>
+  <si>
+    <t>__eq__</t>
+  </si>
+  <si>
+    <t>__getattr__</t>
+  </si>
+  <si>
+    <t>__getitem__</t>
+  </si>
+  <si>
+    <t>__init__</t>
+  </si>
+  <si>
+    <t>__int__</t>
+  </si>
+  <si>
+    <t>__len__</t>
+  </si>
+  <si>
+    <t>__module__</t>
+  </si>
+  <si>
+    <t>__ne__</t>
+  </si>
+  <si>
+    <t>__nonzero__</t>
+  </si>
+  <si>
+    <t>__repr__</t>
+  </si>
+  <si>
+    <t>__setattr__</t>
+  </si>
+  <si>
+    <t>__setitem__</t>
+  </si>
+  <si>
+    <t>__str__</t>
+  </si>
+  <si>
+    <t>_builtMethods_</t>
+  </si>
+  <si>
+    <t>_enum_</t>
+  </si>
+  <si>
+    <t>_find_dispatch_type_</t>
+  </si>
+  <si>
+    <t>_get_good_object_</t>
+  </si>
+  <si>
+    <t>_get_good_single_object_</t>
+  </si>
+  <si>
+    <t>_lazydata_</t>
+  </si>
+  <si>
+    <t>_make_method_</t>
+  </si>
+  <si>
+    <t>_mapCachedItems_</t>
+  </si>
+  <si>
+    <t>_oleobj_</t>
+  </si>
+  <si>
+    <t>_olerepr_</t>
+  </si>
+  <si>
+    <t>_print_details_</t>
+  </si>
+  <si>
+    <t>_proc_</t>
+  </si>
+  <si>
+    <t>_unicode_to_string_</t>
+  </si>
+  <si>
+    <t>_username_</t>
+  </si>
+  <si>
+    <t>_wrap_dispatch_</t>
+  </si>
+  <si>
+    <t>Kierwa</t>
+  </si>
+  <si>
+    <t>Sheet Name</t>
+  </si>
+  <si>
+    <t>Destination Cell</t>
+  </si>
+  <si>
+    <t>Active</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>P4</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>GTO.Rates.List</t>
+  </si>
+  <si>
+    <t>Organization</t>
+  </si>
+  <si>
+    <t>GTO.ABB_Banks.List</t>
+  </si>
+  <si>
+    <t>GTO</t>
+  </si>
+  <si>
+    <t>Torge</t>
+  </si>
+  <si>
+    <t>Roman</t>
+  </si>
+  <si>
+    <t>Atkinson</t>
+  </si>
+  <si>
+    <t>Jaro</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>X3</t>
+  </si>
+  <si>
+    <t>SNL Banks</t>
+  </si>
+  <si>
+    <t>List of banks we received from SNL</t>
+  </si>
+  <si>
+    <t>Adirondack Trust Company</t>
+  </si>
+  <si>
+    <t>AFFIN Bank Bhd.</t>
+  </si>
+  <si>
+    <t>AFFIN Holdings Bhd.</t>
+  </si>
+  <si>
+    <t>Agrani Bank Limited</t>
+  </si>
+  <si>
+    <t>Agricultural Bank of China Limited</t>
+  </si>
+  <si>
+    <t>Agricultural Bank of Taiwan Corporation</t>
+  </si>
+  <si>
+    <t>Agroindustrijska komercijalna banka a.d. Niš</t>
+  </si>
+  <si>
+    <t>Aichi Bank, Ltd.</t>
+  </si>
+  <si>
+    <t>AJS Bancorp, Inc.</t>
+  </si>
+  <si>
+    <t>Akbank TAS</t>
+  </si>
+  <si>
+    <t>Akita Bank, Ltd.</t>
+  </si>
+  <si>
+    <t>Aktia Bank Plc</t>
+  </si>
+  <si>
+    <t>Al Rayan Bank Plc</t>
+  </si>
+  <si>
+    <t>Alamogordo Financial Corp. (MHC)</t>
+  </si>
+  <si>
+    <t>Ålandsbanken Abp</t>
+  </si>
+  <si>
+    <t>Albaraka Türk Katilim Bankasi AS</t>
+  </si>
+  <si>
+    <t>Alerus Financial Corporation</t>
+  </si>
+  <si>
+    <t>ALETTI &amp; C. Banca di Investimento Mobiliare SpA</t>
+  </si>
+  <si>
+    <t>Alior Bank SA</t>
+  </si>
+  <si>
+    <t>Allahabad Bank</t>
+  </si>
+  <si>
+    <t>Allegheny Valley Bancorp, Inc.</t>
+  </si>
+  <si>
+    <t>Allgemeine Sparkasse Oberösterreich Bankaktiengesellschaft</t>
+  </si>
+  <si>
+    <t>Alliance Bancorp, Inc. of Pennsylvania</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -56,16 +323,74 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFD700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF000000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFD700"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -73,14 +398,42 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -360,56 +713,517 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:K18"/>
+  <dimension ref="A1:X28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="35.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D15" t="s">
+      <c r="E3" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="X3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D16" t="s">
+      <c r="B4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="P4" t="s">
+        <v>0</v>
+      </c>
+      <c r="X4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="K16" t="s">
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="P5" t="s">
+        <v>1</v>
+      </c>
+      <c r="X5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="P6" t="s">
+        <v>2</v>
+      </c>
+      <c r="X6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="E7" s="9" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B8" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="17" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D17" t="s">
+      <c r="E8" s="9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>64</v>
+      </c>
+      <c r="B9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>65</v>
+      </c>
+      <c r="B10" t="s">
         <v>5</v>
       </c>
-      <c r="K17" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="K18" t="s">
-        <v>5</v>
+      <c r="E10" s="9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>66</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="E12" s="9" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="E13" s="9" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="E14" s="9" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="E15" s="9" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="E16" s="9" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="17" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E17" s="9" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="18" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E18" s="9" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="19" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E19" s="9" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="20" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E20" s="9" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="21" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E21" s="9" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="22" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E22" s="9" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="23" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E23" s="9" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="24" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E24" s="9" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="25" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E25" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="P25" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="26" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="P26" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="27" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="P27" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="28" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="P28" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B4" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet3"/>
+  <dimension ref="A1:AT14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="95" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="B7" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="J14" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K14" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="L14" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="M14" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="N14" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="O14" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="P14" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q14" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="R14" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="S14" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="T14" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="U14" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="V14" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="W14" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="X14" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y14" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z14" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA14" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB14" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="AC14" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="AD14" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="AE14" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="AF14" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AG14" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="AH14" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AI14" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="AJ14" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AK14" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="AL14" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="AM14" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="AN14" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="AO14" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="AP14" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="AQ14" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="AR14" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="AS14" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="AT14" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B4" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>